<commit_message>
Santa Claus partialy fixed 3
</commit_message>
<xml_diff>
--- a/Лист Microsoft Office Excel.xlsx
+++ b/Лист Microsoft Office Excel.xlsx
@@ -96,37 +96,7 @@
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="7">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -497,8 +467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K5890"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
-      <selection activeCell="C167" sqref="C167"/>
+    <sheetView tabSelected="1" topLeftCell="A190" workbookViewId="0">
+      <selection activeCell="M204" sqref="M204"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -565,7 +535,7 @@
       </c>
       <c r="I4">
         <f>COUNTIF(G3:G5846,"!!!!")</f>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -4100,7 +4070,7 @@
         <v>185</v>
       </c>
       <c r="C187">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E187" s="3" t="s">
         <v>5</v>
@@ -4119,7 +4089,7 @@
         <v>186</v>
       </c>
       <c r="C188">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E188" s="3" t="s">
         <v>6</v>
@@ -4138,7 +4108,7 @@
         <v>187</v>
       </c>
       <c r="C189">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E189" s="3" t="s">
         <v>0</v>
@@ -4157,7 +4127,7 @@
         <v>188</v>
       </c>
       <c r="C190">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E190" s="3" t="s">
         <v>1</v>
@@ -4176,7 +4146,7 @@
         <v>189</v>
       </c>
       <c r="C191">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E191" s="3" t="s">
         <v>2</v>
@@ -4195,7 +4165,7 @@
         <v>190</v>
       </c>
       <c r="C192">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E192" s="3" t="s">
         <v>3</v>
@@ -4214,7 +4184,7 @@
         <v>191</v>
       </c>
       <c r="C193">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E193" s="3" t="s">
         <v>4</v>
@@ -4233,7 +4203,7 @@
         <v>192</v>
       </c>
       <c r="C194">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E194" s="3" t="s">
         <v>5</v>
@@ -4252,7 +4222,7 @@
         <v>193</v>
       </c>
       <c r="C195">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E195" s="3" t="s">
         <v>6</v>
@@ -4271,7 +4241,7 @@
         <v>194</v>
       </c>
       <c r="C196">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E196" s="3" t="s">
         <v>0</v>
@@ -4290,7 +4260,7 @@
         <v>195</v>
       </c>
       <c r="C197">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E197" s="3" t="s">
         <v>1</v>
@@ -4309,7 +4279,7 @@
         <v>196</v>
       </c>
       <c r="C198">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E198" s="3" t="s">
         <v>2</v>
@@ -4328,7 +4298,7 @@
         <v>197</v>
       </c>
       <c r="C199">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E199" s="3" t="s">
         <v>3</v>
@@ -4347,7 +4317,7 @@
         <v>198</v>
       </c>
       <c r="C200">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E200" s="3" t="s">
         <v>4</v>
@@ -4366,7 +4336,7 @@
         <v>199</v>
       </c>
       <c r="C201">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E201" s="3" t="s">
         <v>5</v>
@@ -4385,7 +4355,7 @@
         <v>200</v>
       </c>
       <c r="C202">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E202" s="3" t="s">
         <v>6</v>
@@ -4404,7 +4374,7 @@
         <v>201</v>
       </c>
       <c r="C203">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E203" s="3" t="s">
         <v>0</v>
@@ -4423,7 +4393,7 @@
         <v>202</v>
       </c>
       <c r="C204">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E204" s="3" t="s">
         <v>1</v>
@@ -4442,7 +4412,7 @@
         <v>203</v>
       </c>
       <c r="C205">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E205" s="3" t="s">
         <v>2</v>
@@ -4461,7 +4431,7 @@
         <v>204</v>
       </c>
       <c r="C206">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E206" s="3" t="s">
         <v>3</v>
@@ -4480,7 +4450,7 @@
         <v>205</v>
       </c>
       <c r="C207">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E207" s="3" t="s">
         <v>4</v>
@@ -4499,7 +4469,7 @@
         <v>206</v>
       </c>
       <c r="C208">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E208" s="3" t="s">
         <v>5</v>
@@ -4518,7 +4488,7 @@
         <v>207</v>
       </c>
       <c r="C209">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E209" s="3" t="s">
         <v>6</v>
@@ -4537,7 +4507,7 @@
         <v>208</v>
       </c>
       <c r="C210">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E210" s="3" t="s">
         <v>0</v>
@@ -4556,7 +4526,7 @@
         <v>209</v>
       </c>
       <c r="C211">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E211" s="3" t="s">
         <v>1</v>
@@ -4575,7 +4545,7 @@
         <v>210</v>
       </c>
       <c r="C212">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E212" s="3" t="s">
         <v>2</v>
@@ -4594,7 +4564,7 @@
         <v>211</v>
       </c>
       <c r="C213">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E213" s="3" t="s">
         <v>3</v>
@@ -4613,7 +4583,7 @@
         <v>212</v>
       </c>
       <c r="C214">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E214" s="3" t="s">
         <v>4</v>
@@ -4632,7 +4602,7 @@
         <v>213</v>
       </c>
       <c r="C215">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E215" s="3" t="s">
         <v>5</v>
@@ -4654,7 +4624,7 @@
         <v>214</v>
       </c>
       <c r="C216">
-        <v>31</v>
+        <v>1</v>
       </c>
       <c r="E216" s="3" t="s">
         <v>6</v>
@@ -4673,7 +4643,7 @@
         <v>215</v>
       </c>
       <c r="C217">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E217" s="3" t="s">
         <v>0</v>
@@ -4692,7 +4662,7 @@
         <v>216</v>
       </c>
       <c r="C218">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E218" s="3" t="s">
         <v>1</v>
@@ -4711,7 +4681,7 @@
         <v>217</v>
       </c>
       <c r="C219">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E219" s="3" t="s">
         <v>2</v>
@@ -4730,7 +4700,7 @@
         <v>218</v>
       </c>
       <c r="C220">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E220" s="3" t="s">
         <v>3</v>
@@ -4749,7 +4719,7 @@
         <v>219</v>
       </c>
       <c r="C221">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E221" s="3" t="s">
         <v>4</v>
@@ -4768,7 +4738,7 @@
         <v>220</v>
       </c>
       <c r="C222">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E222" s="3" t="s">
         <v>5</v>
@@ -4787,7 +4757,7 @@
         <v>221</v>
       </c>
       <c r="C223">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E223" s="3" t="s">
         <v>6</v>
@@ -4806,7 +4776,7 @@
         <v>222</v>
       </c>
       <c r="C224">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E224" s="3" t="s">
         <v>0</v>
@@ -4825,7 +4795,7 @@
         <v>223</v>
       </c>
       <c r="C225">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E225" s="3" t="s">
         <v>1</v>
@@ -4844,7 +4814,7 @@
         <v>224</v>
       </c>
       <c r="C226">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E226" s="3" t="s">
         <v>2</v>
@@ -4863,7 +4833,7 @@
         <v>225</v>
       </c>
       <c r="C227">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E227" s="3" t="s">
         <v>3</v>
@@ -4882,7 +4852,7 @@
         <v>226</v>
       </c>
       <c r="C228">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E228" s="3" t="s">
         <v>4</v>
@@ -4891,9 +4861,9 @@
         <f t="shared" si="6"/>
         <v>пт</v>
       </c>
-      <c r="G228" t="b">
+      <c r="G228" t="str">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>!!!!</v>
       </c>
     </row>
     <row r="229" spans="2:7">
@@ -4901,7 +4871,7 @@
         <v>227</v>
       </c>
       <c r="C229">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E229" s="3" t="s">
         <v>5</v>
@@ -4920,7 +4890,7 @@
         <v>228</v>
       </c>
       <c r="C230">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E230" s="3" t="s">
         <v>6</v>
@@ -4939,7 +4909,7 @@
         <v>229</v>
       </c>
       <c r="C231">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E231" s="3" t="s">
         <v>0</v>
@@ -4958,7 +4928,7 @@
         <v>230</v>
       </c>
       <c r="C232">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E232" s="3" t="s">
         <v>1</v>
@@ -4977,7 +4947,7 @@
         <v>231</v>
       </c>
       <c r="C233">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E233" s="3" t="s">
         <v>2</v>
@@ -4996,7 +4966,7 @@
         <v>232</v>
       </c>
       <c r="C234">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E234" s="3" t="s">
         <v>3</v>
@@ -5015,7 +4985,7 @@
         <v>233</v>
       </c>
       <c r="C235">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E235" s="3" t="s">
         <v>4</v>
@@ -5034,7 +5004,7 @@
         <v>234</v>
       </c>
       <c r="C236">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E236" s="3" t="s">
         <v>5</v>
@@ -5053,7 +5023,7 @@
         <v>235</v>
       </c>
       <c r="C237">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E237" s="3" t="s">
         <v>6</v>
@@ -5072,7 +5042,7 @@
         <v>236</v>
       </c>
       <c r="C238">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E238" s="3" t="s">
         <v>0</v>
@@ -5091,7 +5061,7 @@
         <v>237</v>
       </c>
       <c r="C239">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E239" s="3" t="s">
         <v>1</v>
@@ -5110,7 +5080,7 @@
         <v>238</v>
       </c>
       <c r="C240">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E240" s="3" t="s">
         <v>2</v>
@@ -5129,7 +5099,7 @@
         <v>239</v>
       </c>
       <c r="C241">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E241" s="3" t="s">
         <v>3</v>
@@ -5148,7 +5118,7 @@
         <v>240</v>
       </c>
       <c r="C242">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E242" s="3" t="s">
         <v>4</v>
@@ -5167,7 +5137,7 @@
         <v>241</v>
       </c>
       <c r="C243">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E243" s="3" t="s">
         <v>5</v>
@@ -5186,7 +5156,7 @@
         <v>242</v>
       </c>
       <c r="C244">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E244" s="3" t="s">
         <v>6</v>
@@ -5205,7 +5175,7 @@
         <v>243</v>
       </c>
       <c r="C245">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E245" s="3" t="s">
         <v>0</v>
@@ -5224,7 +5194,7 @@
         <v>244</v>
       </c>
       <c r="C246">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E246" s="3" t="s">
         <v>1</v>
@@ -95815,17 +95785,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E3:F5846">
-    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="сб">
+    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="сб">
       <formula>NOT(ISERROR(SEARCH("сб",E3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C5846">
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
       <formula>13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G5846">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
       <formula>"!!!!"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>